<commit_message>
Criado Entities de Usuarios - Editados os strings de todas as class
</commit_message>
<xml_diff>
--- a/SmallRoad/Trunk/Docs/atividades.xlsx
+++ b/SmallRoad/Trunk/Docs/atividades.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\ProjetosAcademicos\SmallRoad\Trunk\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="19095" windowHeight="11010"/>
   </bookViews>
@@ -136,8 +141,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,13 +334,21 @@
       <color rgb="FF008000"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -373,9 +386,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,9 +420,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,9 +472,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -616,14 +665,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A23" sqref="A23:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
@@ -634,7 +683,7 @@
     <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -644,7 +693,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -664,7 +713,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -677,13 +726,13 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -694,13 +743,13 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -711,13 +760,13 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -736,7 +785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -755,7 +804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -769,7 +818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
@@ -786,7 +835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -803,7 +852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -820,7 +869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -837,7 +886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -854,7 +903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -868,7 +917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -882,7 +931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -896,7 +945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -910,7 +959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -921,10 +970,10 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -938,7 +987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -952,7 +1001,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
@@ -966,7 +1015,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
@@ -977,10 +1026,10 @@
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Implementação básica do login.
</commit_message>
<xml_diff>
--- a/SmallRoad/Trunk/Docs/atividades.xlsx
+++ b/SmallRoad/Trunk/Docs/atividades.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\ProjetosAcademicos\SmallRoad\Trunk\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="132" windowWidth="19092" windowHeight="11016"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="19095" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Atividades - DEV Small Road" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
   <si>
     <t>Tela de login</t>
   </si>
@@ -136,13 +131,46 @@
   </si>
   <si>
     <t>Recuperar senha</t>
+  </si>
+  <si>
+    <t>Hygor</t>
+  </si>
+  <si>
+    <t>Cancelado</t>
+  </si>
+  <si>
+    <t>Front-end Tela de login</t>
+  </si>
+  <si>
+    <t>Front-end Tela de cadastro/alteração de usuário</t>
+  </si>
+  <si>
+    <t>Front-end Tela de recuperação de senha</t>
+  </si>
+  <si>
+    <t>Front-end Tela de cadastro/alteração de veículo</t>
+  </si>
+  <si>
+    <t>Front-end Tela de cadastro/alteração de nota fiscal</t>
+  </si>
+  <si>
+    <t>Front-end Tela de listagem/exclusão das notas fiscais</t>
+  </si>
+  <si>
+    <t>Front-end Tela de gerenciamento de roteiro</t>
+  </si>
+  <si>
+    <t>Front-end Tela do mapa</t>
+  </si>
+  <si>
+    <t>Front-end Tela de visualização dos roteiros (para o gerente)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,7 +306,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font>
         <b/>
@@ -326,6 +354,18 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -348,7 +388,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -386,9 +426,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,10 +460,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -455,10 +494,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -631,25 +669,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5546875" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -659,7 +697,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -679,7 +717,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -698,7 +736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -715,7 +753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -726,13 +764,13 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -751,7 +789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -764,13 +802,13 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -783,10 +821,13 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
@@ -799,11 +840,8 @@
       <c r="F9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -817,10 +855,10 @@
         <v>25</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -834,10 +872,10 @@
         <v>25</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -851,10 +889,10 @@
         <v>25</v>
       </c>
       <c r="K12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -865,13 +903,13 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -884,8 +922,11 @@
       <c r="F14" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -898,116 +939,265 @@
       <c r="F15" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="4" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D17" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D19" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D20" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D21" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D22" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D23" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5">
+        <v>2</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5">
+        <v>3</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1016,26 +1206,29 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:F23">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="F3:F32">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"Cancelado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Testes de desenvolvimento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Pausado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F23">
-      <formula1>$K$9:$K$13</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F32">
+      <formula1>$K$10:$K$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C23">
-      <formula1>$K$3:$K$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C32">
+      <formula1>$K$3:$K$8</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Implementação inicial da tela de roteiro do motorista.
</commit_message>
<xml_diff>
--- a/SmallRoad/Trunk/Docs/atividades.xlsx
+++ b/SmallRoad/Trunk/Docs/atividades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>Tela de login</t>
   </si>
@@ -673,7 +673,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -741,7 +741,9 @@
         <v>5</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
       </c>

</xml_diff>